<commit_message>
add Potential graph data
</commit_message>
<xml_diff>
--- a/experience/Potential/graph/result_graph.xlsx
+++ b/experience/Potential/graph/result_graph.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="330" windowWidth="16995" windowHeight="11610"/>
+    <workbookView xWindow="720" yWindow="330" windowWidth="16995" windowHeight="11610" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="chain_N2_4" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="chain_full" sheetId="2" r:id="rId2"/>
+    <sheet name="chain_del" sheetId="3" r:id="rId3"/>
+    <sheet name="tsumoList_D3_D3FULL_D4" sheetId="7" r:id="rId4"/>
+    <sheet name="totalPuyo_D3Del" sheetId="9" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="7">
   <si>
     <t>n=2</t>
     <phoneticPr fontId="1"/>
@@ -27,6 +29,22 @@
   </si>
   <si>
     <t>n=4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>n=3, full width</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>n=4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>n=3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>n=3, delete</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -380,7 +398,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B150"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51:B100"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
@@ -1592,12 +1612,1213 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B150"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A35" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A37" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A38" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A39" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A40" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A41" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A42" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A43" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A44" t="s">
+        <v>1</v>
+      </c>
+      <c r="B44">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A45" t="s">
+        <v>1</v>
+      </c>
+      <c r="B45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A46" t="s">
+        <v>1</v>
+      </c>
+      <c r="B46">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A47" t="s">
+        <v>1</v>
+      </c>
+      <c r="B47">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A48" t="s">
+        <v>1</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A49" t="s">
+        <v>1</v>
+      </c>
+      <c r="B49">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A50" t="s">
+        <v>1</v>
+      </c>
+      <c r="B50">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A51" t="s">
+        <v>3</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A52" t="s">
+        <v>3</v>
+      </c>
+      <c r="B52">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A53" t="s">
+        <v>3</v>
+      </c>
+      <c r="B53">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A54" t="s">
+        <v>3</v>
+      </c>
+      <c r="B54">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A55" t="s">
+        <v>3</v>
+      </c>
+      <c r="B55">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A56" t="s">
+        <v>3</v>
+      </c>
+      <c r="B56">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A57" t="s">
+        <v>3</v>
+      </c>
+      <c r="B57">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A58" t="s">
+        <v>3</v>
+      </c>
+      <c r="B58">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A59" t="s">
+        <v>3</v>
+      </c>
+      <c r="B59">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A60" t="s">
+        <v>3</v>
+      </c>
+      <c r="B60">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A61" t="s">
+        <v>3</v>
+      </c>
+      <c r="B61">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A62" t="s">
+        <v>3</v>
+      </c>
+      <c r="B62">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A63" t="s">
+        <v>3</v>
+      </c>
+      <c r="B63">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A64" t="s">
+        <v>3</v>
+      </c>
+      <c r="B64">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A65" t="s">
+        <v>3</v>
+      </c>
+      <c r="B65">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A66" t="s">
+        <v>3</v>
+      </c>
+      <c r="B66">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A67" t="s">
+        <v>3</v>
+      </c>
+      <c r="B67">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A68" t="s">
+        <v>3</v>
+      </c>
+      <c r="B68">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A69" t="s">
+        <v>3</v>
+      </c>
+      <c r="B69">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A70" t="s">
+        <v>3</v>
+      </c>
+      <c r="B70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A71" t="s">
+        <v>3</v>
+      </c>
+      <c r="B71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A72" t="s">
+        <v>3</v>
+      </c>
+      <c r="B72">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A73" t="s">
+        <v>3</v>
+      </c>
+      <c r="B73">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A74" t="s">
+        <v>3</v>
+      </c>
+      <c r="B74">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A75" t="s">
+        <v>3</v>
+      </c>
+      <c r="B75">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A76" t="s">
+        <v>3</v>
+      </c>
+      <c r="B76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A77" t="s">
+        <v>3</v>
+      </c>
+      <c r="B77">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A78" t="s">
+        <v>3</v>
+      </c>
+      <c r="B78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A79" t="s">
+        <v>3</v>
+      </c>
+      <c r="B79">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A80" t="s">
+        <v>3</v>
+      </c>
+      <c r="B80">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A81" t="s">
+        <v>3</v>
+      </c>
+      <c r="B81">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A82" t="s">
+        <v>3</v>
+      </c>
+      <c r="B82">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A83" t="s">
+        <v>3</v>
+      </c>
+      <c r="B83">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A84" t="s">
+        <v>3</v>
+      </c>
+      <c r="B84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A85" t="s">
+        <v>3</v>
+      </c>
+      <c r="B85">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A86" t="s">
+        <v>3</v>
+      </c>
+      <c r="B86">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A87" t="s">
+        <v>3</v>
+      </c>
+      <c r="B87">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A88" t="s">
+        <v>3</v>
+      </c>
+      <c r="B88">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A89" t="s">
+        <v>3</v>
+      </c>
+      <c r="B89">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A90" t="s">
+        <v>3</v>
+      </c>
+      <c r="B90">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A91" t="s">
+        <v>3</v>
+      </c>
+      <c r="B91">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A92" t="s">
+        <v>3</v>
+      </c>
+      <c r="B92">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A93" t="s">
+        <v>3</v>
+      </c>
+      <c r="B93">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A94" t="s">
+        <v>3</v>
+      </c>
+      <c r="B94">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A95" t="s">
+        <v>3</v>
+      </c>
+      <c r="B95">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A96" t="s">
+        <v>3</v>
+      </c>
+      <c r="B96">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A97" t="s">
+        <v>3</v>
+      </c>
+      <c r="B97">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A98" t="s">
+        <v>3</v>
+      </c>
+      <c r="B98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A99" t="s">
+        <v>3</v>
+      </c>
+      <c r="B99">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A100" t="s">
+        <v>3</v>
+      </c>
+      <c r="B100">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A101" t="s">
+        <v>4</v>
+      </c>
+      <c r="B101">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A102" t="s">
+        <v>4</v>
+      </c>
+      <c r="B102">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A103" t="s">
+        <v>4</v>
+      </c>
+      <c r="B103">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A104" t="s">
+        <v>4</v>
+      </c>
+      <c r="B104">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A105" t="s">
+        <v>4</v>
+      </c>
+      <c r="B105">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A106" t="s">
+        <v>4</v>
+      </c>
+      <c r="B106">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A107" t="s">
+        <v>4</v>
+      </c>
+      <c r="B107">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A108" t="s">
+        <v>4</v>
+      </c>
+      <c r="B108">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A109" t="s">
+        <v>4</v>
+      </c>
+      <c r="B109">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A110" t="s">
+        <v>4</v>
+      </c>
+      <c r="B110">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A111" t="s">
+        <v>4</v>
+      </c>
+      <c r="B111">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A112" t="s">
+        <v>4</v>
+      </c>
+      <c r="B112">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A113" t="s">
+        <v>4</v>
+      </c>
+      <c r="B113">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A114" t="s">
+        <v>4</v>
+      </c>
+      <c r="B114">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A115" t="s">
+        <v>4</v>
+      </c>
+      <c r="B115">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A116" t="s">
+        <v>4</v>
+      </c>
+      <c r="B116">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A117" t="s">
+        <v>4</v>
+      </c>
+      <c r="B117">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A118" t="s">
+        <v>4</v>
+      </c>
+      <c r="B118">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A119" t="s">
+        <v>4</v>
+      </c>
+      <c r="B119">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A120" t="s">
+        <v>4</v>
+      </c>
+      <c r="B120">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A121" t="s">
+        <v>4</v>
+      </c>
+      <c r="B121">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A122" t="s">
+        <v>4</v>
+      </c>
+      <c r="B122">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A123" t="s">
+        <v>4</v>
+      </c>
+      <c r="B123">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A124" t="s">
+        <v>4</v>
+      </c>
+      <c r="B124">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A125" t="s">
+        <v>4</v>
+      </c>
+      <c r="B125">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A126" t="s">
+        <v>4</v>
+      </c>
+      <c r="B126">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A127" t="s">
+        <v>4</v>
+      </c>
+      <c r="B127">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A128" t="s">
+        <v>4</v>
+      </c>
+      <c r="B128">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A129" t="s">
+        <v>4</v>
+      </c>
+      <c r="B129">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A130" t="s">
+        <v>4</v>
+      </c>
+      <c r="B130">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A131" t="s">
+        <v>4</v>
+      </c>
+      <c r="B131">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A132" t="s">
+        <v>4</v>
+      </c>
+      <c r="B132">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A133" t="s">
+        <v>4</v>
+      </c>
+      <c r="B133">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A134" t="s">
+        <v>4</v>
+      </c>
+      <c r="B134">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A135" t="s">
+        <v>4</v>
+      </c>
+      <c r="B135">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A136" t="s">
+        <v>4</v>
+      </c>
+      <c r="B136">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A137" t="s">
+        <v>4</v>
+      </c>
+      <c r="B137">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A138" t="s">
+        <v>4</v>
+      </c>
+      <c r="B138">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A139" t="s">
+        <v>4</v>
+      </c>
+      <c r="B139">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A140" t="s">
+        <v>4</v>
+      </c>
+      <c r="B140">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A141" t="s">
+        <v>4</v>
+      </c>
+      <c r="B141">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A142" t="s">
+        <v>4</v>
+      </c>
+      <c r="B142">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A143" t="s">
+        <v>4</v>
+      </c>
+      <c r="B143">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A144" t="s">
+        <v>4</v>
+      </c>
+      <c r="B144">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A145" t="s">
+        <v>4</v>
+      </c>
+      <c r="B145">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A146" t="s">
+        <v>4</v>
+      </c>
+      <c r="B146">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A147" t="s">
+        <v>4</v>
+      </c>
+      <c r="B147">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A148" t="s">
+        <v>4</v>
+      </c>
+      <c r="B148">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A149" t="s">
+        <v>4</v>
+      </c>
+      <c r="B149">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A150" t="s">
+        <v>4</v>
+      </c>
+      <c r="B150">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1605,12 +2826,1567 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B100"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A37" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A39" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A40" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A42" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A43" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A44" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A45" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A46" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A48" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A49" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A50" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A51" t="s">
+        <v>6</v>
+      </c>
+      <c r="B51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A52" t="s">
+        <v>6</v>
+      </c>
+      <c r="B52">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A53" t="s">
+        <v>6</v>
+      </c>
+      <c r="B53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A54" t="s">
+        <v>6</v>
+      </c>
+      <c r="B54">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A55" t="s">
+        <v>6</v>
+      </c>
+      <c r="B55">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A56" t="s">
+        <v>6</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A57" t="s">
+        <v>6</v>
+      </c>
+      <c r="B57">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A58" t="s">
+        <v>6</v>
+      </c>
+      <c r="B58">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A59" t="s">
+        <v>6</v>
+      </c>
+      <c r="B59">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A60" t="s">
+        <v>6</v>
+      </c>
+      <c r="B60">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A61" t="s">
+        <v>6</v>
+      </c>
+      <c r="B61">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A62" t="s">
+        <v>6</v>
+      </c>
+      <c r="B62">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A63" t="s">
+        <v>6</v>
+      </c>
+      <c r="B63">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A64" t="s">
+        <v>6</v>
+      </c>
+      <c r="B64">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A65" t="s">
+        <v>6</v>
+      </c>
+      <c r="B65">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A66" t="s">
+        <v>6</v>
+      </c>
+      <c r="B66">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A67" t="s">
+        <v>6</v>
+      </c>
+      <c r="B67">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A68" t="s">
+        <v>6</v>
+      </c>
+      <c r="B68">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A69" t="s">
+        <v>6</v>
+      </c>
+      <c r="B69">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A70" t="s">
+        <v>6</v>
+      </c>
+      <c r="B70">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A71" t="s">
+        <v>6</v>
+      </c>
+      <c r="B71">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A72" t="s">
+        <v>6</v>
+      </c>
+      <c r="B72">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A73" t="s">
+        <v>6</v>
+      </c>
+      <c r="B73">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A74" t="s">
+        <v>6</v>
+      </c>
+      <c r="B74">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A75" t="s">
+        <v>6</v>
+      </c>
+      <c r="B75">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A76" t="s">
+        <v>6</v>
+      </c>
+      <c r="B76">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A77" t="s">
+        <v>6</v>
+      </c>
+      <c r="B77">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A78" t="s">
+        <v>6</v>
+      </c>
+      <c r="B78">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A79" t="s">
+        <v>6</v>
+      </c>
+      <c r="B79">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A80" t="s">
+        <v>6</v>
+      </c>
+      <c r="B80">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A81" t="s">
+        <v>6</v>
+      </c>
+      <c r="B81">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A82" t="s">
+        <v>6</v>
+      </c>
+      <c r="B82">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A83" t="s">
+        <v>6</v>
+      </c>
+      <c r="B83">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A84" t="s">
+        <v>6</v>
+      </c>
+      <c r="B84">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A85" t="s">
+        <v>6</v>
+      </c>
+      <c r="B85">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A86" t="s">
+        <v>6</v>
+      </c>
+      <c r="B86">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A87" t="s">
+        <v>6</v>
+      </c>
+      <c r="B87">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A88" t="s">
+        <v>6</v>
+      </c>
+      <c r="B88">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A89" t="s">
+        <v>6</v>
+      </c>
+      <c r="B89">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A90" t="s">
+        <v>6</v>
+      </c>
+      <c r="B90">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A91" t="s">
+        <v>6</v>
+      </c>
+      <c r="B91">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A92" t="s">
+        <v>6</v>
+      </c>
+      <c r="B92">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A93" t="s">
+        <v>6</v>
+      </c>
+      <c r="B93">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A94" t="s">
+        <v>6</v>
+      </c>
+      <c r="B94">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A95" t="s">
+        <v>6</v>
+      </c>
+      <c r="B95">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A96" t="s">
+        <v>6</v>
+      </c>
+      <c r="B96">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A97" t="s">
+        <v>6</v>
+      </c>
+      <c r="B97">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A98" t="s">
+        <v>6</v>
+      </c>
+      <c r="B98">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A99" t="s">
+        <v>6</v>
+      </c>
+      <c r="B99">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A100" t="s">
+        <v>6</v>
+      </c>
+      <c r="B100">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>18.920000000000002</v>
+      </c>
+      <c r="C1">
+        <v>18.920000000000002</v>
+      </c>
+      <c r="D1">
+        <v>18.88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>15.2</v>
+      </c>
+      <c r="C2">
+        <v>16.239999999999998</v>
+      </c>
+      <c r="D2">
+        <v>13.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>13.82</v>
+      </c>
+      <c r="C3">
+        <v>10.039999999999999</v>
+      </c>
+      <c r="D3">
+        <v>10.38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>11.2</v>
+      </c>
+      <c r="C4">
+        <v>5.54</v>
+      </c>
+      <c r="D4">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>10.92</v>
+      </c>
+      <c r="C5">
+        <v>4.68</v>
+      </c>
+      <c r="D5">
+        <v>3.32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>8.14</v>
+      </c>
+      <c r="C6">
+        <v>3.56</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>7.88</v>
+      </c>
+      <c r="C7">
+        <v>3.24</v>
+      </c>
+      <c r="D7">
+        <v>1.98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>5.9</v>
+      </c>
+      <c r="C8">
+        <v>3.08</v>
+      </c>
+      <c r="D8">
+        <v>2.76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>5.92</v>
+      </c>
+      <c r="C9">
+        <v>2.92</v>
+      </c>
+      <c r="D9">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>4.62</v>
+      </c>
+      <c r="C10">
+        <v>3.04</v>
+      </c>
+      <c r="D10">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>3.92</v>
+      </c>
+      <c r="C11">
+        <v>2.62</v>
+      </c>
+      <c r="D11">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>4.28</v>
+      </c>
+      <c r="C12">
+        <v>2.38</v>
+      </c>
+      <c r="D12">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="C13">
+        <v>2.8</v>
+      </c>
+      <c r="D13">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>3.22</v>
+      </c>
+      <c r="C14">
+        <v>2.52</v>
+      </c>
+      <c r="D14">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>2.98</v>
+      </c>
+      <c r="C15">
+        <v>1.78</v>
+      </c>
+      <c r="D15">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>3.48</v>
+      </c>
+      <c r="C16">
+        <v>2.36</v>
+      </c>
+      <c r="D16">
+        <v>1.66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>3.38</v>
+      </c>
+      <c r="C17">
+        <v>2.5</v>
+      </c>
+      <c r="D17">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>2.84</v>
+      </c>
+      <c r="C18">
+        <v>2.52</v>
+      </c>
+      <c r="D18">
+        <v>1.94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>4.22</v>
+      </c>
+      <c r="C19">
+        <v>1.94</v>
+      </c>
+      <c r="D19">
+        <v>1.86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>2.74</v>
+      </c>
+      <c r="C20">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="D20">
+        <v>1.84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>3.5</v>
+      </c>
+      <c r="C21">
+        <v>2.04</v>
+      </c>
+      <c r="D21">
+        <v>1.82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A22">
+        <v>22</v>
+      </c>
+      <c r="B22">
+        <v>3.3</v>
+      </c>
+      <c r="C22">
+        <v>2.66</v>
+      </c>
+      <c r="D22">
+        <v>1.52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="B23">
+        <v>3.34</v>
+      </c>
+      <c r="C23">
+        <v>2.74</v>
+      </c>
+      <c r="D23">
+        <v>1.54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A24">
+        <v>24</v>
+      </c>
+      <c r="B24">
+        <v>2.54</v>
+      </c>
+      <c r="C24">
+        <v>2.6</v>
+      </c>
+      <c r="D24">
+        <v>1.46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <v>2.76</v>
+      </c>
+      <c r="C25">
+        <v>2.7</v>
+      </c>
+      <c r="D25">
+        <v>1.66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A26">
+        <v>26</v>
+      </c>
+      <c r="B26">
+        <v>2.84</v>
+      </c>
+      <c r="C26">
+        <v>1.86</v>
+      </c>
+      <c r="D26">
+        <v>1.58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A27">
+        <v>27</v>
+      </c>
+      <c r="B27">
+        <v>2.88</v>
+      </c>
+      <c r="C27">
+        <v>2.08</v>
+      </c>
+      <c r="D27">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A28">
+        <v>28</v>
+      </c>
+      <c r="B28">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="C28">
+        <v>1.84</v>
+      </c>
+      <c r="D28">
+        <v>1.68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A29">
+        <v>29</v>
+      </c>
+      <c r="B29">
+        <v>2.72</v>
+      </c>
+      <c r="C29">
+        <v>2.44</v>
+      </c>
+      <c r="D29">
+        <v>1.48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A30">
+        <v>30</v>
+      </c>
+      <c r="B30">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="C30">
+        <v>1.98</v>
+      </c>
+      <c r="D30">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A31">
+        <v>31</v>
+      </c>
+      <c r="B31">
+        <v>2.76</v>
+      </c>
+      <c r="C31">
+        <v>2.02</v>
+      </c>
+      <c r="D31">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A32">
+        <v>32</v>
+      </c>
+      <c r="B32">
+        <v>2.16</v>
+      </c>
+      <c r="C32">
+        <v>1.94</v>
+      </c>
+      <c r="D32">
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A33">
+        <v>33</v>
+      </c>
+      <c r="B33">
+        <v>1.2</v>
+      </c>
+      <c r="C33">
+        <v>1.26</v>
+      </c>
+      <c r="D33">
+        <v>1.08</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>5.92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>7.92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>9.2799999999999994</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>11.04</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>12.96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>14.88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>16.079999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>17.38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>18.64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>19.88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>21.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>22.76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>24.3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>25.68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>26.54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>27.7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>28.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>29.36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>30.6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A22">
+        <v>22</v>
+      </c>
+      <c r="B22">
+        <v>30.82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="B23">
+        <v>32.380000000000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A24">
+        <v>24</v>
+      </c>
+      <c r="B24">
+        <v>33.159999999999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <v>33.44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A26">
+        <v>26</v>
+      </c>
+      <c r="B26">
+        <v>34.380000000000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A27">
+        <v>27</v>
+      </c>
+      <c r="B27">
+        <v>35.4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A28">
+        <v>28</v>
+      </c>
+      <c r="B28">
+        <v>36.08</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A29">
+        <v>29</v>
+      </c>
+      <c r="B29">
+        <v>37.04</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A30">
+        <v>30</v>
+      </c>
+      <c r="B30">
+        <v>37.380000000000003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A31">
+        <v>31</v>
+      </c>
+      <c r="B31">
+        <v>38.72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A32">
+        <v>32</v>
+      </c>
+      <c r="B32">
+        <v>38.380000000000003</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A33">
+        <v>33</v>
+      </c>
+      <c r="B33">
+        <v>37.26</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>